<commit_message>
* Added SimulationImtVale object for IMT_VALE simulation scenario
</commit_message>
<xml_diff>
--- a/sharc/parameters/bs_data/brucuCCO2600.xlsx
+++ b/sharc/parameters/bs_data/brucuCCO2600.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19017"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\OICE_16_974FA576_32C1D314_27E9\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bfaria/source/SHARC_SON/SHARC/sharc/parameters/bs_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="962EC4593EE27C617B62A7D1924A970F2B0C893E" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{2F4F93B9-F613-A046-BD05-19D1593E3252}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3140" yWindow="4460" windowWidth="20500" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171026"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -92,7 +92,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -405,18 +405,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="9" max="9" width="8.5703125" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" customWidth="1"/>
-    <col min="14" max="14" width="16.28515625" customWidth="1"/>
+    <col min="9" max="9" width="8.5" customWidth="1"/>
+    <col min="13" max="13" width="14.5" customWidth="1"/>
+    <col min="14" max="14" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,7 +463,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -489,7 +489,7 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>43.616999999999997</v>
+        <v>0</v>
       </c>
       <c r="J2">
         <v>2600</v>
@@ -510,7 +510,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -536,7 +536,7 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="J3">
         <v>2600</v>

</xml_diff>